<commit_message>
Write the timedata to the xlsx
</commit_message>
<xml_diff>
--- a/Konsulttidrapport-Responsive-2020-02.xlsx
+++ b/Konsulttidrapport-Responsive-2020-02.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-9720" windowWidth="16440" windowHeight="28440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Januari 2019" sheetId="1" state="visible" r:id="rId1"/>
@@ -419,8 +419,8 @@
   </sheetPr>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" s="17" t="inlineStr">
         <is>
-          <t>Thomas Nilefalk</t>
+          <t>&lt;user&gt;</t>
         </is>
       </c>
       <c r="O2" s="1" t="n"/>
@@ -909,9 +909,7 @@
       <c r="A22" s="5" t="n">
         <v>43876</v>
       </c>
-      <c r="B22" s="6" t="n">
-        <v>6</v>
-      </c>
+      <c r="B22" s="6" t="n"/>
       <c r="C22" s="6" t="n"/>
       <c r="D22" s="6" t="n"/>
       <c r="E22" s="6" t="n"/>
@@ -1057,9 +1055,7 @@
       <c r="A28" s="5" t="n">
         <v>43882</v>
       </c>
-      <c r="B28" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="B28" s="6" t="n"/>
       <c r="C28" s="6" t="n"/>
       <c r="D28" s="6" t="n"/>
       <c r="E28" s="6" t="n"/>
@@ -1127,7 +1123,7 @@
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>4:30</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="C31" s="6" t="n"/>
@@ -1153,7 +1149,7 @@
       </c>
       <c r="B32" s="6" t="inlineStr">
         <is>
-          <t>2:30</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="C32" s="6" t="n"/>
@@ -1179,7 +1175,7 @@
       </c>
       <c r="B33" s="6" t="inlineStr">
         <is>
-          <t>6:30</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="C33" s="6" t="n"/>
@@ -1323,8 +1319,9 @@
           <t>summa per projekt</t>
         </is>
       </c>
-      <c r="B39" s="11" t="n">
-        <v>12</v>
+      <c r="B39" s="11">
+        <f>SUM(B8:B38)</f>
+        <v/>
       </c>
       <c r="C39" s="11" t="n"/>
       <c r="D39" s="11" t="n"/>

</xml_diff>